<commit_message>
Simplified Testing Code Removed a bug in testing code Updated speed files
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldo\IdeaProjects\bitsorter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2873EF24-60F8-4805-B8B4-CFCA582D47FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBE2C6C-FEF2-4798-BB33-622735009B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{531A9B83-56C7-409E-96BA-E7D8F7323E1F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>2022-12</t>
   </si>
@@ -103,6 +103,12 @@
   <si>
     <t>JavaSorterMTObjectInt</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2023-01</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -158,6 +164,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,6 +642,135 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-223E-463E-9511-AC210B52BD81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$62:$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>QuickBitSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MixedBitSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RadixBitSorterMTInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$62:$E$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2691-4956-978F-357A284C344F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1397,6 +1533,129 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$78:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterObjectInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JavaSorterMTObjectInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RadixBitSorterObjectInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$78:$E$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5416</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F950-4124-B867-4E719466433F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
@@ -2186,6 +2445,141 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-79BB-4DC0-BEBC-E00F00ED61EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$52:$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>QuickBitSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RadixBitSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RadixByteSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>JavaSorterMTInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$52:$E$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2486</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-302F-4140-AA83-753F0B4DE9FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4556,6 +4950,141 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$27:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>QuickBitSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RadixBitSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RadixByteSorterInt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>JavaSorterMTInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$27:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6ACE-4FB7-A4AC-FEAFA10953C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
@@ -5336,6 +5865,135 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6CFA-46CC-9534-8BD4116928B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$37:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>QuickBitSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MixedBitSorterMTInt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RadixBitSorterMTInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$37:$E$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DCA-4287-BA49-D1FB1DF6B542}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6101,6 +6759,129 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-DFAC-492C-AC1B-96A8CE4B0146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Positive!$E$88</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2023-01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Positive!$A$89:$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>JavaSorterObjectInt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JavaSorterMTObjectInt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RadixBitSorterObjectInt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Positive!$E$89:$E$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4089</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-79D7-4C36-A251-BEE4AA3D92C5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14129,16 +14910,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14310,15 +15091,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:colOff>769620</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14635,7 +15416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -14645,8 +15426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39B731E-57F4-47F9-B805-D8A8C5A5FE8D}">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C131" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -14656,12 +15437,12 @@
     <col min="3" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -14671,8 +15452,11 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -14686,7 +15470,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -14700,7 +15484,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -14714,7 +15498,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -14728,7 +15512,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -14742,7 +15526,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -14756,7 +15540,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -14770,7 +15554,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -14784,7 +15568,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="B12" t="str">
         <f>B2</f>
         <v>2022-02</v>
@@ -14798,84 +15582,84 @@
         <v>2022-12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="str">
-        <f>A7</f>
+        <f t="shared" ref="A13:D16" si="0">A7</f>
         <v>JavaSorterMTInt</v>
       </c>
       <c r="B13">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="C13">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="D13">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>QuickBitSorterMTInt</v>
       </c>
       <c r="B14">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="C14">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="D14">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>MixedBitSorterMTInt</v>
       </c>
       <c r="B15">
-        <f>B9</f>
+        <f t="shared" si="0"/>
         <v>98</v>
       </c>
       <c r="C15">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="D15">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>RadixBitSorterMTInt</v>
       </c>
       <c r="B16">
-        <f>B10</f>
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="C16">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="D16">
-        <f>D10</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -14885,8 +15669,11 @@
       <c r="D26" t="s">
         <v>0</v>
       </c>
+      <c r="E26" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -14899,8 +15686,11 @@
       <c r="D27">
         <v>541</v>
       </c>
+      <c r="E27">
+        <v>524</v>
+      </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -14913,8 +15703,11 @@
       <c r="D28">
         <v>54</v>
       </c>
+      <c r="E28">
+        <v>44</v>
+      </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -14927,8 +15720,11 @@
       <c r="D29">
         <v>85</v>
       </c>
+      <c r="E29">
+        <v>75</v>
+      </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -14941,8 +15737,11 @@
       <c r="D30">
         <v>111</v>
       </c>
+      <c r="E30">
+        <v>90</v>
+      </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -14955,8 +15754,11 @@
       <c r="D31">
         <v>81</v>
       </c>
+      <c r="E31">
+        <v>72</v>
+      </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -14969,8 +15771,11 @@
       <c r="D32">
         <v>54</v>
       </c>
+      <c r="E32">
+        <v>45</v>
+      </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -14983,8 +15788,11 @@
       <c r="D33">
         <v>48</v>
       </c>
+      <c r="E33">
+        <v>39</v>
+      </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -14997,8 +15805,11 @@
       <c r="D34">
         <v>54</v>
       </c>
+      <c r="E34">
+        <v>41</v>
+      </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="B36" t="str">
         <f>B26</f>
         <v>2022-04</v>
@@ -15011,85 +15822,105 @@
         <f>D26</f>
         <v>2022-12</v>
       </c>
+      <c r="E36" t="str">
+        <f>E26</f>
+        <v>2023-01</v>
+      </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="str">
-        <f>A31</f>
+        <f t="shared" ref="A37:D40" si="1">A31</f>
         <v>JavaSorterMTInt</v>
       </c>
       <c r="B37">
-        <f>B31</f>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="C37">
-        <f>C31</f>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="D37">
-        <f>D31</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
+      <c r="E37">
+        <f t="shared" ref="E37" si="2">E31</f>
+        <v>72</v>
+      </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="str">
-        <f>A32</f>
+        <f t="shared" si="1"/>
         <v>QuickBitSorterMTInt</v>
       </c>
       <c r="B38">
-        <f>B32</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C38">
-        <f>C32</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="D38">
-        <f>D32</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
+      <c r="E38">
+        <f t="shared" ref="E38" si="3">E32</f>
+        <v>45</v>
+      </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="str">
-        <f>A33</f>
+        <f t="shared" si="1"/>
         <v>MixedBitSorterMTInt</v>
       </c>
       <c r="B39">
-        <f>B33</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C39">
-        <f>C33</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="D39">
-        <f>D33</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
+      <c r="E39">
+        <f t="shared" ref="E39" si="4">E33</f>
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="str">
-        <f>A34</f>
+        <f t="shared" si="1"/>
         <v>RadixBitSorterMTInt</v>
       </c>
       <c r="B40">
-        <f>B34</f>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="C40">
-        <f>C34</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="D40">
-        <f>D34</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
+      <c r="E40">
+        <f t="shared" ref="E40" si="5">E34</f>
+        <v>41</v>
+      </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:5">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -15099,8 +15930,11 @@
       <c r="D51" t="s">
         <v>0</v>
       </c>
+      <c r="E51" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -15113,8 +15947,11 @@
       <c r="D52">
         <v>3174</v>
       </c>
+      <c r="E52">
+        <v>3096</v>
+      </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -15127,8 +15964,11 @@
       <c r="D53">
         <v>2593</v>
       </c>
+      <c r="E53">
+        <v>2486</v>
+      </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -15141,8 +15981,11 @@
       <c r="D54">
         <v>474</v>
       </c>
+      <c r="E54">
+        <v>433</v>
+      </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -15152,8 +15995,11 @@
       <c r="D55">
         <v>505</v>
       </c>
+      <c r="E55">
+        <v>439</v>
+      </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -15166,8 +16012,11 @@
       <c r="D56">
         <v>365</v>
       </c>
+      <c r="E56">
+        <v>353</v>
+      </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -15180,8 +16029,11 @@
       <c r="D57">
         <v>589</v>
       </c>
+      <c r="E57">
+        <v>583</v>
+      </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -15194,8 +16046,11 @@
       <c r="D58">
         <v>449</v>
       </c>
+      <c r="E58">
+        <v>379</v>
+      </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -15208,8 +16063,11 @@
       <c r="D59">
         <v>289</v>
       </c>
+      <c r="E59">
+        <v>252</v>
+      </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:5">
       <c r="B61" t="str">
         <f>B51</f>
         <v>2022-03</v>
@@ -15222,85 +16080,105 @@
         <f>D51</f>
         <v>2022-12</v>
       </c>
+      <c r="E61" t="str">
+        <f>E51</f>
+        <v>2023-01</v>
+      </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:5">
       <c r="A62" t="str">
-        <f>A56</f>
+        <f t="shared" ref="A62:E65" si="6">A56</f>
         <v>JavaSorterMTInt</v>
       </c>
       <c r="B62">
-        <f>B56</f>
+        <f t="shared" si="6"/>
         <v>410</v>
       </c>
       <c r="C62">
-        <f>C56</f>
+        <f t="shared" si="6"/>
         <v>406</v>
       </c>
       <c r="D62">
-        <f>D56</f>
+        <f t="shared" si="6"/>
         <v>365</v>
       </c>
+      <c r="E62">
+        <f t="shared" si="6"/>
+        <v>353</v>
+      </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:5">
       <c r="A63" t="str">
-        <f>A57</f>
+        <f t="shared" si="6"/>
         <v>QuickBitSorterMTInt</v>
       </c>
       <c r="B63">
-        <f>B57</f>
+        <f t="shared" si="6"/>
         <v>657</v>
       </c>
       <c r="C63">
-        <f>C57</f>
+        <f t="shared" si="6"/>
         <v>578</v>
       </c>
       <c r="D63">
-        <f>D57</f>
+        <f t="shared" si="6"/>
         <v>589</v>
       </c>
+      <c r="E63">
+        <f t="shared" si="6"/>
+        <v>583</v>
+      </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:5">
       <c r="A64" t="str">
-        <f>A58</f>
+        <f t="shared" si="6"/>
         <v>MixedBitSorterMTInt</v>
       </c>
       <c r="B64">
-        <f>B58</f>
+        <f t="shared" si="6"/>
         <v>664</v>
       </c>
       <c r="C64">
-        <f>C58</f>
+        <f t="shared" si="6"/>
         <v>571</v>
       </c>
       <c r="D64">
-        <f>D58</f>
+        <f t="shared" si="6"/>
         <v>449</v>
       </c>
+      <c r="E64">
+        <f t="shared" si="6"/>
+        <v>379</v>
+      </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="str">
-        <f>A59</f>
+        <f t="shared" si="6"/>
         <v>RadixBitSorterMTInt</v>
       </c>
       <c r="B65">
-        <f>B59</f>
+        <f t="shared" si="6"/>
         <v>397</v>
       </c>
       <c r="C65">
-        <f>C59</f>
+        <f t="shared" si="6"/>
         <v>372</v>
       </c>
       <c r="D65">
-        <f>D59</f>
+        <f t="shared" si="6"/>
         <v>289</v>
       </c>
+      <c r="E65">
+        <f t="shared" si="6"/>
+        <v>252</v>
+      </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="B77" t="s">
         <v>16</v>
       </c>
@@ -15310,8 +16188,11 @@
       <c r="D77" t="s">
         <v>0</v>
       </c>
+      <c r="E77" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
         <v>20</v>
       </c>
@@ -15324,8 +16205,11 @@
       <c r="D78">
         <v>5584</v>
       </c>
+      <c r="E78">
+        <v>5416</v>
+      </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
         <v>21</v>
       </c>
@@ -15338,8 +16222,11 @@
       <c r="D79">
         <v>717</v>
       </c>
+      <c r="E79">
+        <v>691</v>
+      </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -15352,13 +16239,16 @@
       <c r="D80">
         <v>813</v>
       </c>
+      <c r="E80">
+        <v>965</v>
+      </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:5">
       <c r="B88" t="s">
         <v>16</v>
       </c>
@@ -15368,8 +16258,11 @@
       <c r="D88" t="s">
         <v>0</v>
       </c>
+      <c r="E88" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
         <v>20</v>
       </c>
@@ -15382,8 +16275,11 @@
       <c r="D89">
         <v>4450</v>
       </c>
+      <c r="E89">
+        <v>4089</v>
+      </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:5">
       <c r="A90" s="2" t="s">
         <v>21</v>
       </c>
@@ -15396,8 +16292,11 @@
       <c r="D90">
         <v>826</v>
       </c>
+      <c r="E90">
+        <v>637</v>
+      </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
         <v>17</v>
       </c>
@@ -15409,6 +16308,9 @@
       </c>
       <c r="D91">
         <v>644</v>
+      </c>
+      <c r="E91">
+        <v>608</v>
       </c>
     </row>
     <row r="118" spans="1:7">

</xml_diff>